<commit_message>
petites modif gnucash + pdf
</commit_message>
<xml_diff>
--- a/3 - Suivi Actifs (T)/2-Comptes de Caisses/2023-2024/Autres /blackfreeday_castor_241123.xlsx
+++ b/3 - Suivi Actifs (T)/2-Comptes de Caisses/2023-2024/Autres /blackfreeday_castor_241123.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianmanzini/Desktop/Unipoly/UPSecretrariat/3 - Suivi Actifs (T)/2-Comptes de Caisses/2023-2024/Autres /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07296A81-1431-1C44-8E63-00A67CB53F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B0910-33FD-FA45-9BFA-ECE8EE8E4F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$CHF-100C]&quot; &quot;#,##0.00;[Red][$CHF-100C]&quot; -&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-100C]General"/>
@@ -303,24 +303,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="18">
-    <cellStyle name="Accent" xfId="2"/>
-    <cellStyle name="Accent 1" xfId="3"/>
-    <cellStyle name="Accent 2" xfId="4"/>
-    <cellStyle name="Accent 3" xfId="5"/>
-    <cellStyle name="Bad" xfId="6"/>
-    <cellStyle name="Error" xfId="7"/>
-    <cellStyle name="Footnote" xfId="8"/>
-    <cellStyle name="Good" xfId="9"/>
-    <cellStyle name="Heading" xfId="10"/>
-    <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Heading 2" xfId="12"/>
-    <cellStyle name="Hyperlink" xfId="13"/>
-    <cellStyle name="Neutral" xfId="14"/>
+    <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Error" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Good" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Heading" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading 1" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Hyperlink" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Neutral" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="1" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+    <cellStyle name="Status" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Text" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Warning" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -631,12 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.1640625" style="9" customWidth="1"/>
     <col min="2" max="2" width="1.6640625" style="2" customWidth="1"/>
@@ -657,7 +659,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:1024" ht="14">
+    <row r="2" spans="1:1024">
       <c r="A2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -674,7 +676,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" ht="14">
+    <row r="4" spans="1:1024">
       <c r="A4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1817,20 +1819,24 @@
       <c r="A14" s="7">
         <v>20</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
       <c r="E14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="18" customHeight="1">
       <c r="A15" s="7">
         <v>50</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
       <c r="E15" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:1024" ht="18" customHeight="1">
@@ -1863,33 +1869,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14"/>
     <row r="20" spans="1:5" ht="21">
       <c r="D20" s="11">
         <f>SUM(E6:E18)</f>
-        <v>191.7</v>
+        <v>261.7</v>
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="14"/>
-    <row r="22" spans="1:5" ht="14">
+    <row r="22" spans="1:5">
       <c r="C22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5" ht="14">
+    <row r="23" spans="1:5">
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:5" ht="14">
+    <row r="24" spans="1:5">
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5" ht="14">
+    <row r="25" spans="1:5">
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>

</xml_diff>